<commit_message>
area estimation pipeline stage, small visualization modifs
</commit_message>
<xml_diff>
--- a/modules/area_estimation/ScalingFactor.xlsx
+++ b/modules/area_estimation/ScalingFactor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\GitHub\ai-pothole-models\deployment\modules\area_estimation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\GitHub\ai-pothole-models\modules\area_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A1910B-3097-4AA7-AE30-E9F38D9A5166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789BDDF3-8822-498D-B11A-DC4479FA115E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Rectangle</t>
   </si>
@@ -126,6 +126,18 @@
   <si>
     <t>y-axis distance from camera
 (pixels)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -133,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="207" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -178,12 +190,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -192,8 +198,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -201,7 +211,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +399,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CA"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -460,7 +472,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -675,7 +686,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CA"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1628,7 +1639,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1644,34 +1655,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
@@ -1697,7 +1708,7 @@
         <f>0.5*0.5</f>
         <v>0.25</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="6">
         <f>G3/F3</f>
         <v>1.1098247009688326E-7</v>
       </c>
@@ -1726,8 +1737,8 @@
         <f t="shared" ref="G4:G9" si="0">0.5*0.5</f>
         <v>0.25</v>
       </c>
-      <c r="H4" s="10">
-        <f t="shared" ref="H4:J9" si="1">G4/F4</f>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H9" si="1">G4/F4</f>
         <v>3.3379619739371929E-6</v>
       </c>
     </row>
@@ -1735,10 +1746,10 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1006</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1755,20 +1766,20 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="6">
         <f t="shared" si="1"/>
         <v>1.3354700854700855E-5</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>941</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1785,20 +1796,20 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="6">
         <f t="shared" si="1"/>
         <v>3.908692933083177E-5</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>900</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1815,20 +1826,20 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="6">
         <f t="shared" si="1"/>
         <v>1.0121457489878542E-4</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>873</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1845,20 +1856,20 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="6">
         <f t="shared" si="1"/>
         <v>1.8037518037518038E-4</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>854</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1875,144 +1886,119 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="6">
         <f t="shared" si="1"/>
         <v>3.2051282051282051E-4</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>1972</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <v>1.1098247009688326E-7</v>
       </c>
-      <c r="F17" s="10">
-        <f xml:space="preserve"> -0.0002278815 / (-249.575444 + 0.6036185*C17 + -0.000365585*C17*C17)</f>
-        <v>4.7384407425525229E-7</v>
+      <c r="F17" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="G17">
-        <f>ABS((D17-F17)/D17)</f>
-        <v>3.2695398096799009</v>
+        <v>-2.2788150560381401E-4</v>
+      </c>
+      <c r="H17">
+        <f>G17/(G18+G19*(2297)+G20*(2297*2297))</f>
+        <v>2.8774128597886977E-7</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>1158</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <v>3.3379619739371929E-6</v>
       </c>
-      <c r="F18" s="10">
-        <f t="shared" ref="F18:F23" si="2" xml:space="preserve"> -0.0002278815 / (-249.575444 + 0.6036185*C18 + -0.000365585*C18*C18)</f>
-        <v>5.5823830365789072E-6</v>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G23" si="3">ABS((D18-F18)/D18)</f>
-        <v>0.67239263963045537</v>
+        <v>-249.575444271701</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C19" s="4">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C19" s="2">
         <v>1006</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <v>1.3354700854700855E-5</v>
       </c>
-      <c r="F19" s="10">
-        <f t="shared" si="2"/>
-        <v>1.8496253363744383E-5</v>
+      <c r="F19" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>0.38499945187717943</v>
+        <v>0.60361848274124597</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C20" s="4">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C20" s="2">
         <v>941</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="6">
         <v>3.908692933083177E-5</v>
       </c>
-      <c r="F20" s="10">
-        <f t="shared" si="2"/>
-        <v>4.308587698123178E-5</v>
+      <c r="F20" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>0.10230907668783386</v>
+        <v>-3.6558500089469299E-4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C21" s="4">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C21" s="2">
         <v>900</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="6">
         <v>1.0121457489878542E-4</v>
       </c>
-      <c r="F21" s="10">
-        <f t="shared" si="2"/>
-        <v>9.3292964508946818E-5</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
-        <v>7.8265510651605391E-2</v>
-      </c>
+      <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C22" s="4">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C22" s="2">
         <v>873</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>1.8037518037518038E-4</v>
       </c>
-      <c r="F22" s="10">
-        <f t="shared" si="2"/>
-        <v>1.8386081472935442E-4</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>1.9324356859540912E-2</v>
-      </c>
+      <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C23" s="4">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C23" s="2">
         <v>854</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="6">
         <v>3.2051282051282051E-4</v>
       </c>
-      <c r="F23" s="10">
-        <f t="shared" si="2"/>
-        <v>3.199527470475012E-4</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
-        <v>1.747429211796255E-3</v>
-      </c>
+      <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="D24" s="3"/>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="D25" s="3"/>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="D26" s="3"/>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="D27" s="3"/>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D27" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
created initial depth estimation stage (added DepthAnythingV2 files)
</commit_message>
<xml_diff>
--- a/modules/area_estimation/ScalingFactor.xlsx
+++ b/modules/area_estimation/ScalingFactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\GitHub\ai-pothole-models\modules\area_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789BDDF3-8822-498D-B11A-DC4479FA115E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1F49B-9C1E-4174-A1E1-E83C57652CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Rectangle</t>
   </si>
@@ -108,14 +108,6 @@
  centre of rectangle (pixels)</t>
   </si>
   <si>
-    <t>Bounding box area
-(pixels)</t>
-  </si>
-  <si>
-    <t>Actual bounding box area
-(m2)</t>
-  </si>
-  <si>
     <t>Scaling Factor Needed
 (m2/pixel)</t>
   </si>
@@ -138,6 +130,18 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Bounding box area
+(pixel^2)</t>
+  </si>
+  <si>
+    <t>Actual bounding box area
+(m^2)</t>
+  </si>
+  <si>
+    <t>Scaling Factor Needed
+(m^2/pixel^2)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,6 +206,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -211,9 +218,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,6 +251,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Scaling Factor Needed
+(m2/pixel2)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1639,7 +1670,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1655,8 +1686,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
@@ -1666,20 +1697,20 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="10"/>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1894,10 +1925,10 @@
     </row>
     <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
         <v>25</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1908,15 +1939,15 @@
       <c r="D17" s="6">
         <v>1.1098247009688326E-7</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>28</v>
+      <c r="F17" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G17">
         <v>-2.2788150560381401E-4</v>
       </c>
       <c r="H17">
-        <f>G17/(G18+G19*(2297)+G20*(2297*2297))</f>
-        <v>2.8774128597886977E-7</v>
+        <f>G17/(G18+G19*(C3)+G20*(C3*C3))</f>
+        <v>4.7384404867829322E-7</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.45">
@@ -1926,8 +1957,8 @@
       <c r="D18" s="6">
         <v>3.3379619739371929E-6</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>29</v>
+      <c r="F18" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="G18">
         <v>-249.575444271701</v>
@@ -1940,8 +1971,8 @@
       <c r="D19" s="6">
         <v>1.3354700854700855E-5</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>30</v>
+      <c r="F19" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="G19">
         <v>0.60361848274124597</v>
@@ -1954,8 +1985,8 @@
       <c r="D20" s="6">
         <v>3.908692933083177E-5</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>31</v>
+      <c r="F20" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="G20">
         <v>-3.6558500089469299E-4</v>

</xml_diff>